<commit_message>
Typo voor 2.1... :) Artiest in plaats van docent.
</commit_message>
<xml_diff>
--- a/productbacklog webshop cursussen.xlsx
+++ b/productbacklog webshop cursussen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bertjansen/Documents/vsa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bertjansen/Documents/vsa herverlee/repos/vsa-heverlee-nj2020-cursussen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E29F3A-206E-B44B-9613-4F36B1844F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BE698DF-25EB-5A4A-8189-640419851FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" xr2:uid="{162AA7BA-1B78-784A-AFED-773F724E36D9}"/>
   </bookViews>
@@ -473,9 +473,6 @@
     <t>11.4</t>
   </si>
   <si>
-    <t>Een cursus omvat een naam, artiest,  beeld, datum/uur (begin/eind), locatie, omschrijving, in verkoop, gepubliceerd, (early-bird) prijs en een max. hoeveelheid beschikbare inschrijvingen</t>
-  </si>
-  <si>
     <t>zoeken op naam, docent, datum, categorie</t>
   </si>
   <si>
@@ -513,6 +510,9 @@
   </si>
   <si>
     <t>op voorwaarde dat er geen inschrijving is gekoppeld aan de cursus</t>
+  </si>
+  <si>
+    <t>Een cursus omvat een naam, docent,  beeld, datum/uur (begin/eind), locatie, omschrijving, in verkoop, gepubliceerd, (early-bird) prijs en een max. hoeveelheid beschikbare inschrijvingen</t>
   </si>
 </sst>
 </file>
@@ -981,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8F293D-A62C-E74D-853F-4851E1C8B084}">
   <dimension ref="A1:AA991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="186" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="186" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1280,7 +1280,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>3</v>
@@ -1289,7 +1289,7 @@
         <v>107</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
@@ -1327,7 +1327,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>3</v>
@@ -1417,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>3</v>
@@ -2798,7 +2798,7 @@
       <c r="H42" s="8"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -2878,7 +2878,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
@@ -2977,7 +2977,7 @@
       <c r="H47" s="8"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
@@ -3013,7 +3013,7 @@
         <v>2</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H48" s="8"/>
       <c r="I48" s="14"/>
@@ -3052,7 +3052,7 @@
         <v>2</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="14"/>
@@ -3091,7 +3091,7 @@
         <v>2</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:27" ht="17" x14ac:dyDescent="0.2">
@@ -3110,7 +3110,7 @@
         <v>2</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H51" s="8"/>
       <c r="I51" s="14"/>
@@ -3133,7 +3133,7 @@
       <c r="Z51" s="8"/>
       <c r="AA51" s="8"/>
     </row>
-    <row r="52" spans="1:27" ht="29" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" ht="43" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
         <v>100</v>
       </c>
@@ -3149,12 +3149,12 @@
         <v>2</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
@@ -3353,7 +3353,7 @@
       <c r="Z57" s="8"/>
       <c r="AA57" s="8"/>
     </row>
-    <row r="58" spans="1:27" ht="29" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" ht="43" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>145</v>
       </c>
@@ -3374,7 +3374,7 @@
       <c r="H58" s="8"/>
       <c r="I58" s="14"/>
       <c r="J58" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>

</xml_diff>